<commit_message>
Ya subi categoria clientes..fijense para asignar...las categorias
</commit_message>
<xml_diff>
--- a/preveedores_BD.xlsx
+++ b/preveedores_BD.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="proveedores" sheetId="1" r:id="rId1"/>
     <sheet name="empleados" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Condiciones_Venta" sheetId="3" r:id="rId3"/>
+    <sheet name="Categorias_Clientes" sheetId="4" r:id="rId4"/>
+    <sheet name="Niveles_Acceso" sheetId="5" r:id="rId5"/>
+    <sheet name="Cargos" sheetId="6" r:id="rId6"/>
+    <sheet name="IVA_Tasas" sheetId="7" r:id="rId7"/>
+    <sheet name="Depositos" sheetId="8" r:id="rId8"/>
+    <sheet name="Hoja6" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">empleados!$A$1:$F$22</definedName>
@@ -20,29 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="324">
-  <si>
-    <t>NOMBRE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="367">
   <si>
     <t>RUC</t>
   </si>
   <si>
-    <t>DIRECCION</t>
-  </si>
-  <si>
-    <t>TELEFONO</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>SALDO</t>
-  </si>
-  <si>
-    <t>ID_PROVEEDOR</t>
-  </si>
-  <si>
     <t>AB Electricidad</t>
   </si>
   <si>
@@ -667,18 +655,6 @@
     <t>80005674-1</t>
   </si>
   <si>
-    <t>ID_EMPLEADO</t>
-  </si>
-  <si>
-    <t>APELLIDO</t>
-  </si>
-  <si>
-    <t>CEDULA</t>
-  </si>
-  <si>
-    <t>DOMICILIO</t>
-  </si>
-  <si>
     <t xml:space="preserve">Javier Ignacio </t>
   </si>
   <si>
@@ -805,9 +781,6 @@
     <t>Adrian</t>
   </si>
   <si>
-    <t>Sanabria</t>
-  </si>
-  <si>
     <t>Lucia</t>
   </si>
   <si>
@@ -992,6 +965,168 @@
   </si>
   <si>
     <t>Gral. Díaz C/ Agapito Ortiz Paiva 772</t>
+  </si>
+  <si>
+    <t>ID_Condicion</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Contado</t>
+  </si>
+  <si>
+    <t>Crédito</t>
+  </si>
+  <si>
+    <t>ID_Categoria</t>
+  </si>
+  <si>
+    <t>Linea_Credito</t>
+  </si>
+  <si>
+    <t>Mayorista_Tipo_Uno</t>
+  </si>
+  <si>
+    <t>Mayorista_Tipo_Dos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayorista_Tipo_Tres </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayorista_Tipo_Cuatro </t>
+  </si>
+  <si>
+    <t>Minorista</t>
+  </si>
+  <si>
+    <t>ID_Acceso</t>
+  </si>
+  <si>
+    <t>Tipo_Acceso</t>
+  </si>
+  <si>
+    <t>Tipo_1</t>
+  </si>
+  <si>
+    <t>para vendedor</t>
+  </si>
+  <si>
+    <t>Tipo_2</t>
+  </si>
+  <si>
+    <t>para depositero</t>
+  </si>
+  <si>
+    <t>Tipo_3</t>
+  </si>
+  <si>
+    <t>para supervisor</t>
+  </si>
+  <si>
+    <t>Tipo_4</t>
+  </si>
+  <si>
+    <t>para gerente</t>
+  </si>
+  <si>
+    <t>ID_Cargo</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Niveles Acceso</t>
+  </si>
+  <si>
+    <t>Vendedor</t>
+  </si>
+  <si>
+    <t>Depositero</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>Gerente</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Cedula</t>
+  </si>
+  <si>
+    <t>Domicilio</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>ID_Empleado</t>
+  </si>
+  <si>
+    <t>Nombres</t>
+  </si>
+  <si>
+    <t>Apellidos</t>
+  </si>
+  <si>
+    <t>Araujo</t>
+  </si>
+  <si>
+    <t>ID_Proveedor</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Saldo</t>
+  </si>
+  <si>
+    <t>ID_Tasa</t>
+  </si>
+  <si>
+    <t>Porcentaje</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>ID_Deposito</t>
+  </si>
+  <si>
+    <t>Local N° 1</t>
+  </si>
+  <si>
+    <t>Local N° 2</t>
+  </si>
+  <si>
+    <t>Local N° 3</t>
+  </si>
+  <si>
+    <t>ID_Tipo_Pago</t>
+  </si>
+  <si>
+    <t>Efectivo</t>
+  </si>
+  <si>
+    <t>Cheque</t>
+  </si>
+  <si>
+    <t>Nota de Extraccion</t>
+  </si>
+  <si>
+    <t>Pagare</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1072,11 +1207,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1100,6 +1246,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1398,8 +1547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1415,25 +1564,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24.75" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>6</v>
+        <v>349</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>2</v>
+        <v>350</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>3</v>
+        <v>344</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>4</v>
+        <v>351</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>5</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1441,19 +1590,19 @@
         <v>100</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G2" s="3">
         <v>0</v>
@@ -1464,19 +1613,19 @@
         <v>101</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -1487,19 +1636,19 @@
         <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -1510,19 +1659,19 @@
         <v>103</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G5" s="4">
         <v>8000000</v>
@@ -1533,19 +1682,19 @@
         <v>104</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -1556,19 +1705,19 @@
         <v>105</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G7" s="4">
         <v>900000</v>
@@ -1579,19 +1728,19 @@
         <v>106</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G8" s="4">
         <v>700000</v>
@@ -1602,19 +1751,19 @@
         <v>107</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -1625,19 +1774,19 @@
         <v>108</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G10" s="4">
         <v>10000000</v>
@@ -1648,19 +1797,19 @@
         <v>109</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G11" s="4">
         <v>7000000</v>
@@ -1671,19 +1820,19 @@
         <v>110</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G12" s="3">
         <v>0</v>
@@ -1694,19 +1843,19 @@
         <v>111</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G13" s="3">
         <v>0</v>
@@ -1717,19 +1866,19 @@
         <v>112</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G14" s="3">
         <v>0</v>
@@ -1740,19 +1889,19 @@
         <v>113</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G15" s="3">
         <v>0</v>
@@ -1763,19 +1912,19 @@
         <v>114</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G16" s="4">
         <v>30000000</v>
@@ -1786,19 +1935,19 @@
         <v>115</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
@@ -1809,19 +1958,19 @@
         <v>116</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G18" s="4">
         <v>3000000</v>
@@ -1832,19 +1981,19 @@
         <v>117</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G19" s="3">
         <v>0</v>
@@ -1855,19 +2004,19 @@
         <v>118</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G20" s="4">
         <v>540000</v>
@@ -1878,19 +2027,19 @@
         <v>119</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G21" s="3">
         <v>0</v>
@@ -1901,19 +2050,19 @@
         <v>120</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G22" s="3">
         <v>0</v>
@@ -1924,19 +2073,19 @@
         <v>121</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G23" s="4">
         <v>8000000</v>
@@ -1947,19 +2096,19 @@
         <v>122</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G24" s="3">
         <v>0</v>
@@ -1970,19 +2119,19 @@
         <v>123</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G25" s="4">
         <v>900000</v>
@@ -1993,19 +2142,19 @@
         <v>124</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G26" s="3">
         <v>0</v>
@@ -2016,19 +2165,19 @@
         <v>125</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G27" s="3">
         <v>0</v>
@@ -2039,19 +2188,19 @@
         <v>126</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="G28" s="3">
         <v>0</v>
@@ -2062,19 +2211,19 @@
         <v>127</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G29" s="4">
         <v>5000000</v>
@@ -2085,19 +2234,19 @@
         <v>128</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G30" s="4">
         <v>4000000</v>
@@ -2108,19 +2257,19 @@
         <v>129</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G31" s="3">
         <v>0</v>
@@ -2131,19 +2280,19 @@
         <v>130</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G32" s="4">
         <v>300000</v>
@@ -2154,19 +2303,19 @@
         <v>131</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="G33" s="4">
         <v>4000000</v>
@@ -2177,19 +2326,19 @@
         <v>132</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="G34" s="4">
         <v>2000000</v>
@@ -2200,19 +2349,19 @@
         <v>133</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G35" s="3">
         <v>0</v>
@@ -2223,19 +2372,19 @@
         <v>134</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G36" s="4">
         <v>860000</v>
@@ -2246,19 +2395,19 @@
         <v>135</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G37" s="4">
         <v>600000</v>
@@ -2269,19 +2418,19 @@
         <v>136</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G38" s="3">
         <v>0</v>
@@ -2292,19 +2441,19 @@
         <v>137</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G39" s="4">
         <v>1000000</v>
@@ -2315,19 +2464,19 @@
         <v>138</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G40" s="4">
         <v>560000</v>
@@ -2338,19 +2487,19 @@
         <v>139</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G41" s="3">
         <v>0</v>
@@ -2361,19 +2510,19 @@
         <v>140</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G42" s="3">
         <v>0</v>
@@ -2384,19 +2533,19 @@
         <v>141</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G43" s="4">
         <v>900000</v>
@@ -2407,19 +2556,19 @@
         <v>142</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G44" s="6">
         <v>3000000</v>
@@ -2486,10 +2635,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2501,444 +2650,885 @@
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21.75" customHeight="1">
+    <row r="1" spans="1:7" ht="21.75" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>215</v>
+        <v>345</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>0</v>
+        <v>346</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>216</v>
+        <v>347</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>217</v>
+        <v>342</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>218</v>
+        <v>343</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>344</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="9">
         <v>100</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>232</v>
+      </c>
+      <c r="G2" s="8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="9">
         <v>101</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>231</v>
+      </c>
+      <c r="G3" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="9">
         <v>102</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>235</v>
+      </c>
+      <c r="G4" s="8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="9">
         <v>103</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>233</v>
+      </c>
+      <c r="G5" s="8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="9">
         <v>104</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>234</v>
+      </c>
+      <c r="G6" s="8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="9">
         <v>105</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>236</v>
+      </c>
+      <c r="G7" s="8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="9">
         <v>106</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>237</v>
+      </c>
+      <c r="G8" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="9">
         <v>107</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>238</v>
+      </c>
+      <c r="G9" s="8">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="9">
         <v>108</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>239</v>
+      </c>
+      <c r="G10" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="9">
         <v>109</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>240</v>
+      </c>
+      <c r="G11" s="8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="9">
         <v>110</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>241</v>
+      </c>
+      <c r="G12" s="8">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="9">
         <v>111</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>242</v>
+      </c>
+      <c r="G13" s="8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="9">
         <v>112</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>243</v>
+      </c>
+      <c r="G14" s="8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="9">
         <v>113</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>256</v>
+      </c>
+      <c r="G15" s="8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="9">
         <v>114</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>257</v>
+      </c>
+      <c r="G16" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="9">
         <v>115</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>258</v>
+      </c>
+      <c r="G17" s="8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="9">
         <v>116</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>259</v>
+      </c>
+      <c r="G18" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="9">
         <v>117</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>260</v>
+      </c>
+      <c r="G19" s="8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="9">
         <v>118</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="9">
         <v>119</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" s="8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="9">
         <v>120</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>274</v>
+        <v>263</v>
+      </c>
+      <c r="G22" s="8">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21.75" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8">
+        <v>100</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8">
+        <v>101</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21.75" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="8">
+        <v>100</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="8">
+        <v>101</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="8">
+        <v>102</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="C4" s="8">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="8">
+        <v>103</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="C5" s="8">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="8">
+        <v>104</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C6" s="8">
+        <v>11000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21.75" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="8">
+        <v>100</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="8">
+        <v>101</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="8">
+        <v>102</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="8">
+        <v>103</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21.75" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="8">
+        <v>100</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="8">
+        <v>101</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C3" s="8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="8">
+        <v>102</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" s="8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="8">
+        <v>103</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C5" s="8">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21.75" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8">
+        <v>100</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8">
+        <v>101</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8">
+        <v>102</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21.75" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8">
+        <v>100</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8">
+        <v>101</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8">
+        <v>102</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -2946,14 +3536,69 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21.75" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8">
+        <v>100</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8">
+        <v>101</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8">
+        <v>102</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8">
+        <v>103</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>